<commit_message>
Made my own changes
</commit_message>
<xml_diff>
--- a/src/resources/exceldata/Data.xlsx
+++ b/src/resources/exceldata/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fazil\IdeaProjects\AutomationFramework\src\resources\exceldata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9A55034-3087-4091-90CC-8378B6F0091B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EBF0147-BAAB-45D3-BA68-408BEE3B5784}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Player Details" sheetId="1" r:id="rId1"/>
@@ -722,7 +722,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1730,7 +1732,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AC22529-71D5-4ED8-8297-6F0121BF9D42}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -1812,8 +1814,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A72A632B-AA74-49E4-A90B-9581E193B196}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>